<commit_message>
feat(MusicVisualizer): Add song timings
</commit_message>
<xml_diff>
--- a/assets/song-timings/Something-Conforting-Porter-Robinson-Timings.xlsx
+++ b/assets/song-timings/Something-Conforting-Porter-Robinson-Timings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\College\College Files\Code\Year2\CA\Sem2\OOP\MusicVisuals\assets\song-timings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AA308F-3546-46C0-905D-2549AEEC515E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB26CBC6-7C35-4636-BD92-29D7822975E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3165" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,62 +25,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Section Name</t>
   </si>
   <si>
-    <t>Timings</t>
-  </si>
-  <si>
     <t>Intro</t>
   </si>
   <si>
-    <t>0:00 - 0:13</t>
-  </si>
-  <si>
-    <t>0:13 - 0:39</t>
-  </si>
-  <si>
-    <t>0:39 - 0:52</t>
-  </si>
-  <si>
-    <t>0:52 - 1:04</t>
-  </si>
-  <si>
     <t>BuildUp</t>
   </si>
   <si>
     <t>Chours</t>
   </si>
   <si>
-    <t>1:04 - 1:19</t>
-  </si>
-  <si>
-    <t>1:19 - 1:32</t>
-  </si>
-  <si>
     <t>Planned Visual</t>
   </si>
   <si>
-    <t>1:32 - 1:46</t>
-  </si>
-  <si>
     <t>Verse 1</t>
   </si>
   <si>
-    <t>1:46 - 1:53</t>
-  </si>
-  <si>
-    <t>1:53 - 1:58</t>
-  </si>
-  <si>
-    <t>1:58 - 2:12</t>
-  </si>
-  <si>
-    <t>2:12 - 2:25</t>
-  </si>
-  <si>
     <t>SlowBuildUp</t>
   </si>
   <si>
@@ -90,46 +54,19 @@
     <t>Ernest John Decina</t>
   </si>
   <si>
-    <t>2:25 - 2:38</t>
-  </si>
-  <si>
-    <t>2:38 - 2:53</t>
-  </si>
-  <si>
-    <t>2:53 - 3:06</t>
-  </si>
-  <si>
-    <t>3:06 - 3:18</t>
-  </si>
-  <si>
-    <t>3:18 - 3:28</t>
-  </si>
-  <si>
-    <t>3:28 - 3:32</t>
-  </si>
-  <si>
     <t>Bridge</t>
   </si>
   <si>
-    <t>3:32 - 3:46</t>
-  </si>
-  <si>
-    <t>3:46 - 4:00</t>
-  </si>
-  <si>
-    <t>4:00 - 4:12</t>
-  </si>
-  <si>
-    <t>4:12 - 4:20</t>
-  </si>
-  <si>
-    <t>4:20 - 4:26</t>
-  </si>
-  <si>
-    <t>4:26 - 4:41</t>
-  </si>
-  <si>
     <t>Ron Pingol</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>1999</t>
   </si>
 </sst>
 </file>
@@ -165,9 +102,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,195 +386,244 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>135</v>
+      </c>
+      <c r="C3">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4">
+        <v>395</v>
+      </c>
+      <c r="C4">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>530</v>
+      </c>
+      <c r="C5">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B6">
+        <v>667</v>
+      </c>
+      <c r="C6">
+        <v>802</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>802</v>
+      </c>
+      <c r="C7">
+        <v>935</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>935</v>
+      </c>
+      <c r="C8">
+        <v>1075</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B9">
+        <v>1075</v>
+      </c>
+      <c r="C9">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1140</v>
+      </c>
+      <c r="C10">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1198</v>
+      </c>
+      <c r="C11">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>1328</v>
+      </c>
+      <c r="C12">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B13">
+        <v>1465</v>
+      </c>
+      <c r="C13">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>1598</v>
+      </c>
+      <c r="C14">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>1868</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>2094</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>2049</v>
+      </c>
+      <c r="C17">
+        <v>2134</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B18">
+        <v>2134</v>
+      </c>
+      <c r="C18">
+        <v>2262</v>
+      </c>
+      <c r="E18" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>33</v>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>2262</v>
+      </c>
+      <c r="C19">
+        <v>2390</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>2390</v>
+      </c>
+      <c r="C20">
+        <v>2681</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>2681</v>
+      </c>
+      <c r="C21">
+        <v>2770</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(BigBangUniverse): Add drawSphere & drawRings
</commit_message>
<xml_diff>
--- a/assets/song-timings/Something-Conforting-Porter-Robinson-Timings.xlsx
+++ b/assets/song-timings/Something-Conforting-Porter-Robinson-Timings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\College\College Files\Code\Year2\CA\Sem2\OOP\MusicVisuals\assets\song-timings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB26CBC6-7C35-4636-BD92-29D7822975E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61FF2ED-6C72-4276-A2FE-E9CCC5895AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -389,7 +389,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>